<commit_message>
Export Datum transformation added
</commit_message>
<xml_diff>
--- a/CSAY_LatLongUTMToFrom_Converter/CSAY_LatLongUTMToFrom_Converter/bin/Debug/New Microsoft Excel Worksheet.xlsx
+++ b/CSAY_LatLongUTMToFrom_Converter/CSAY_LatLongUTMToFrom_Converter/bin/Debug/New Microsoft Excel Worksheet.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\VBStudio\CSAY_LATLONG_UTM_CONVERTER\CSAY_LatLongUTMToFrom_Converter\CSAY_LatLongUTMToFrom_Converter\bin\Debug\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{147BFE0B-521C-49FB-A1B3-1397600F43F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -18,8 +24,25 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>SN</t>
+  </si>
+  <si>
+    <t>LATITUDE</t>
+  </si>
+  <si>
+    <t>LONGITUDE</t>
+  </si>
+  <si>
+    <t>ELLIPSOIDHEIGHT</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -330,13 +353,614 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>27.445</v>
+      </c>
+      <c r="C2">
+        <v>83.26</v>
+      </c>
+      <c r="D2">
+        <v>42.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>27.446999999999999</v>
+      </c>
+      <c r="C3">
+        <v>83.263000000000005</v>
+      </c>
+      <c r="D3">
+        <f>D2+0.2</f>
+        <v>42.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>27.45</v>
+      </c>
+      <c r="C4">
+        <v>83.256</v>
+      </c>
+      <c r="D4">
+        <f>D3+0.8</f>
+        <v>43.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>27.45</v>
+      </c>
+      <c r="C5">
+        <v>83.254000000000005</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="D5:D40" si="0">D4+0.8</f>
+        <v>44.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>27.449000000000002</v>
+      </c>
+      <c r="C6">
+        <v>83.251999999999995</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>45.099999999999994</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>27.449000000000002</v>
+      </c>
+      <c r="C7">
+        <v>83.25</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>45.899999999999991</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>27.45</v>
+      </c>
+      <c r="C8">
+        <v>83.245999999999995</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>46.699999999999989</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>27.452000000000002</v>
+      </c>
+      <c r="C9">
+        <v>83.24</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>47.499999999999986</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>27.452999999999999</v>
+      </c>
+      <c r="C10">
+        <v>83.236999999999995</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>48.299999999999983</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>27.457000000000001</v>
+      </c>
+      <c r="C11">
+        <v>83.228999999999999</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>49.09999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>27.459</v>
+      </c>
+      <c r="C12">
+        <v>83.221999999999994</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>49.899999999999977</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>27.463000000000001</v>
+      </c>
+      <c r="C13">
+        <v>83.21</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>50.699999999999974</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>27.466999999999999</v>
+      </c>
+      <c r="C14">
+        <v>83.200999999999993</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>51.499999999999972</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>27.466999999999999</v>
+      </c>
+      <c r="C15">
+        <v>83.195999999999998</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>52.299999999999969</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>27.466000000000001</v>
+      </c>
+      <c r="C16">
+        <v>83.188999999999993</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>53.099999999999966</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>27.47</v>
+      </c>
+      <c r="C17">
+        <v>83.180999999999997</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>53.899999999999963</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>27.47</v>
+      </c>
+      <c r="C18">
+        <v>83.177000000000007</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>54.69999999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>27.472000000000001</v>
+      </c>
+      <c r="C19">
+        <v>83.171000000000006</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>55.499999999999957</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>27.471</v>
+      </c>
+      <c r="C20">
+        <v>83.167000000000002</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>56.299999999999955</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>27.471</v>
+      </c>
+      <c r="C21">
+        <v>83.165999999999997</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>57.099999999999952</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>27.472000000000001</v>
+      </c>
+      <c r="C22">
+        <v>83.162999999999997</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>57.899999999999949</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>27.472999999999999</v>
+      </c>
+      <c r="C23">
+        <v>83.161000000000001</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>58.699999999999946</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>27.472999999999999</v>
+      </c>
+      <c r="C24">
+        <v>83.16</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>59.499999999999943</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>27.474</v>
+      </c>
+      <c r="C25">
+        <v>83.156999999999996</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>60.29999999999994</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>27.474</v>
+      </c>
+      <c r="C26">
+        <v>83.153999999999996</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>61.099999999999937</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>27.478000000000002</v>
+      </c>
+      <c r="C27">
+        <v>83.144999999999996</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>61.899999999999935</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>27.478000000000002</v>
+      </c>
+      <c r="C28">
+        <v>83.141999999999996</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>62.699999999999932</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>27.478000000000002</v>
+      </c>
+      <c r="C29">
+        <v>83.141000000000005</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>63.499999999999929</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>27.481000000000002</v>
+      </c>
+      <c r="C30">
+        <v>83.135999999999996</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>64.299999999999926</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>27.481999999999999</v>
+      </c>
+      <c r="C31">
+        <v>83.132000000000005</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>65.099999999999923</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>27.486999999999998</v>
+      </c>
+      <c r="C32">
+        <v>83.126000000000005</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>65.89999999999992</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>27.49</v>
+      </c>
+      <c r="C33">
+        <v>83.123000000000005</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>66.699999999999918</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>27.492999999999999</v>
+      </c>
+      <c r="C34">
+        <v>83.116</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="0"/>
+        <v>67.499999999999915</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>27.495999999999999</v>
+      </c>
+      <c r="C35">
+        <v>83.11</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>68.299999999999912</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>27.498000000000001</v>
+      </c>
+      <c r="C36">
+        <v>83.108999999999995</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="0"/>
+        <v>69.099999999999909</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>27.5</v>
+      </c>
+      <c r="C37">
+        <v>83.103999999999999</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="0"/>
+        <v>69.899999999999906</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>27.501000000000001</v>
+      </c>
+      <c r="C38">
+        <v>83.102999999999994</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="0"/>
+        <v>70.699999999999903</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>27.501999999999999</v>
+      </c>
+      <c r="C39">
+        <v>83.100999999999999</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="0"/>
+        <v>71.499999999999901</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>27.501000000000001</v>
+      </c>
+      <c r="C40">
+        <v>83.1</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="0"/>
+        <v>72.299999999999898</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>